<commit_message>
Added market value functionality and have first working version of class
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -1832,7 +1832,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:RR46"/>
+  <dimension ref="A1:RR47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -68575,7 +68575,7 @@
         <v>0</v>
       </c>
       <c r="MI46">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="MJ46">
         <v>0</v>
@@ -68993,6 +68993,1466 @@
       </c>
       <c r="RR46">
         <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:486">
+      <c r="A47" s="2">
+        <v>43857</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>1.268419838764061</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>2.358713936863353</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>1.638496125706936</v>
+      </c>
+      <c r="I47">
+        <v>25.1261541894969</v>
+      </c>
+      <c r="J47">
+        <v>0.9165119296602739</v>
+      </c>
+      <c r="K47">
+        <v>13.29371723668544</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>0.1464025497482977</v>
+      </c>
+      <c r="O47">
+        <v>8.20246104638511</v>
+      </c>
+      <c r="P47">
+        <v>17.07374710982651</v>
+      </c>
+      <c r="Q47">
+        <v>16.64710303647132</v>
+      </c>
+      <c r="R47">
+        <v>0.1436804500462117</v>
+      </c>
+      <c r="S47">
+        <v>0</v>
+      </c>
+      <c r="T47">
+        <v>0</v>
+      </c>
+      <c r="U47">
+        <v>0.9850927460414027</v>
+      </c>
+      <c r="V47">
+        <v>0</v>
+      </c>
+      <c r="W47">
+        <v>0</v>
+      </c>
+      <c r="X47">
+        <v>1.616170784843689</v>
+      </c>
+      <c r="Y47">
+        <v>3.304059836047912</v>
+      </c>
+      <c r="Z47">
+        <v>0.8517291555195001</v>
+      </c>
+      <c r="AA47">
+        <v>0.8579526519478549</v>
+      </c>
+      <c r="AB47">
+        <v>0</v>
+      </c>
+      <c r="AC47">
+        <v>0</v>
+      </c>
+      <c r="AD47">
+        <v>-107.0858776254204</v>
+      </c>
+      <c r="AE47">
+        <v>1.144110600044883</v>
+      </c>
+      <c r="AF47">
+        <v>98.43219405584477</v>
+      </c>
+      <c r="AG47">
+        <v>2.080364991291731</v>
+      </c>
+      <c r="AH47">
+        <v>9.406551601124818</v>
+      </c>
+      <c r="AI47">
+        <v>0</v>
+      </c>
+      <c r="AJ47">
+        <v>0.008579564785499372</v>
+      </c>
+      <c r="AK47">
+        <v>1.641211167097538</v>
+      </c>
+      <c r="AL47">
+        <v>9.857679230287033</v>
+      </c>
+      <c r="AM47">
+        <v>0</v>
+      </c>
+      <c r="AN47">
+        <v>0</v>
+      </c>
+      <c r="AO47">
+        <v>0</v>
+      </c>
+      <c r="AP47">
+        <v>0</v>
+      </c>
+      <c r="AQ47">
+        <v>22.0343803933103</v>
+      </c>
+      <c r="AR47">
+        <v>4.655858679254465</v>
+      </c>
+      <c r="AS47">
+        <v>0</v>
+      </c>
+      <c r="AT47">
+        <v>1.819952300264561</v>
+      </c>
+      <c r="AU47">
+        <v>0</v>
+      </c>
+      <c r="AV47">
+        <v>0</v>
+      </c>
+      <c r="AW47">
+        <v>3.395836583427013</v>
+      </c>
+      <c r="AX47">
+        <v>5.442271246497171</v>
+      </c>
+      <c r="AY47">
+        <v>34.81575238964069</v>
+      </c>
+      <c r="AZ47">
+        <v>17.40425990141739</v>
+      </c>
+      <c r="BA47">
+        <v>0</v>
+      </c>
+      <c r="BB47">
+        <v>-3.163679351483246</v>
+      </c>
+      <c r="BC47">
+        <v>2.765393963994057</v>
+      </c>
+      <c r="BD47">
+        <v>3.414478491757052</v>
+      </c>
+      <c r="BE47">
+        <v>0</v>
+      </c>
+      <c r="BF47">
+        <v>3.665160490380629</v>
+      </c>
+      <c r="BG47">
+        <v>0.393946620058621</v>
+      </c>
+      <c r="BH47">
+        <v>2.3510078273749</v>
+      </c>
+      <c r="BI47">
+        <v>1.45590942009224</v>
+      </c>
+      <c r="BJ47">
+        <v>1.050593818650505</v>
+      </c>
+      <c r="BK47">
+        <v>0</v>
+      </c>
+      <c r="BL47">
+        <v>1.65302361250707</v>
+      </c>
+      <c r="BM47">
+        <v>54.90287838440236</v>
+      </c>
+      <c r="BN47">
+        <v>-16.61381925252601</v>
+      </c>
+      <c r="BO47">
+        <v>0</v>
+      </c>
+      <c r="BP47">
+        <v>15.00772204252439</v>
+      </c>
+      <c r="BQ47">
+        <v>0.1877693186332436</v>
+      </c>
+      <c r="BR47">
+        <v>-0.763684877859248</v>
+      </c>
+      <c r="BS47">
+        <v>2.999449431736451</v>
+      </c>
+      <c r="BT47">
+        <v>0</v>
+      </c>
+      <c r="BU47">
+        <v>0</v>
+      </c>
+      <c r="BV47">
+        <v>2.632176162880043</v>
+      </c>
+      <c r="BW47">
+        <v>0.9186398063713455</v>
+      </c>
+      <c r="BX47">
+        <v>0.05750638838344679</v>
+      </c>
+      <c r="BY47">
+        <v>1.508084318399497</v>
+      </c>
+      <c r="BZ47">
+        <v>1.579031101077192</v>
+      </c>
+      <c r="CA47">
+        <v>0</v>
+      </c>
+      <c r="CB47">
+        <v>0</v>
+      </c>
+      <c r="CC47">
+        <v>8.532036254643543</v>
+      </c>
+      <c r="CD47">
+        <v>0</v>
+      </c>
+      <c r="CE47">
+        <v>12.81566084858719</v>
+      </c>
+      <c r="CF47">
+        <v>0</v>
+      </c>
+      <c r="CG47">
+        <v>0</v>
+      </c>
+      <c r="CH47">
+        <v>19.17224926885285</v>
+      </c>
+      <c r="CI47">
+        <v>0.3722449905637859</v>
+      </c>
+      <c r="CJ47">
+        <v>10.48636737969889</v>
+      </c>
+      <c r="CK47">
+        <v>0</v>
+      </c>
+      <c r="CL47">
+        <v>3.682434396701979</v>
+      </c>
+      <c r="CM47">
+        <v>4.507505136475174</v>
+      </c>
+      <c r="CN47">
+        <v>0</v>
+      </c>
+      <c r="CO47">
+        <v>0</v>
+      </c>
+      <c r="CP47">
+        <v>0.3173573337822404</v>
+      </c>
+      <c r="CQ47">
+        <v>0</v>
+      </c>
+      <c r="CR47">
+        <v>11.19095550405962</v>
+      </c>
+      <c r="CS47">
+        <v>0</v>
+      </c>
+      <c r="CT47">
+        <v>43.50376528829895</v>
+      </c>
+      <c r="CU47">
+        <v>0</v>
+      </c>
+      <c r="CV47">
+        <v>6.180993899119358</v>
+      </c>
+      <c r="CW47">
+        <v>0</v>
+      </c>
+      <c r="CX47">
+        <v>0</v>
+      </c>
+      <c r="CY47">
+        <v>0</v>
+      </c>
+      <c r="CZ47">
+        <v>0.1232755303126538</v>
+      </c>
+      <c r="DA47">
+        <v>0</v>
+      </c>
+      <c r="DB47">
+        <v>0.2881486938136106</v>
+      </c>
+      <c r="DC47">
+        <v>0</v>
+      </c>
+      <c r="DD47">
+        <v>0</v>
+      </c>
+      <c r="DE47">
+        <v>0</v>
+      </c>
+      <c r="DF47">
+        <v>0</v>
+      </c>
+      <c r="DG47">
+        <v>0</v>
+      </c>
+      <c r="DH47">
+        <v>2.956335600175862</v>
+      </c>
+      <c r="DI47">
+        <v>18.4988975339503</v>
+      </c>
+      <c r="DJ47">
+        <v>0</v>
+      </c>
+      <c r="DK47">
+        <v>0</v>
+      </c>
+      <c r="DL47">
+        <v>4.070164642470672</v>
+      </c>
+      <c r="DM47">
+        <v>0</v>
+      </c>
+      <c r="DN47">
+        <v>-4.831078302068477</v>
+      </c>
+      <c r="DO47">
+        <v>2.98688495368981</v>
+      </c>
+      <c r="DP47">
+        <v>3.351180454461883</v>
+      </c>
+      <c r="DQ47">
+        <v>4.752961451060798</v>
+      </c>
+      <c r="DR47">
+        <v>0</v>
+      </c>
+      <c r="DS47">
+        <v>0</v>
+      </c>
+      <c r="DT47">
+        <v>0</v>
+      </c>
+      <c r="DU47">
+        <v>0</v>
+      </c>
+      <c r="DV47">
+        <v>0</v>
+      </c>
+      <c r="DW47">
+        <v>0</v>
+      </c>
+      <c r="DX47">
+        <v>1.150724968207783</v>
+      </c>
+      <c r="DY47">
+        <v>1.037238854404848</v>
+      </c>
+      <c r="DZ47">
+        <v>0</v>
+      </c>
+      <c r="EA47">
+        <v>4.072231449632454</v>
+      </c>
+      <c r="EB47">
+        <v>0</v>
+      </c>
+      <c r="EC47">
+        <v>59.82858333979311</v>
+      </c>
+      <c r="ED47">
+        <v>0</v>
+      </c>
+      <c r="EE47">
+        <v>0</v>
+      </c>
+      <c r="EF47">
+        <v>-0.9738272266295667</v>
+      </c>
+      <c r="EG47">
+        <v>10.09057669165986</v>
+      </c>
+      <c r="EH47">
+        <v>1.28735113369499</v>
+      </c>
+      <c r="EI47">
+        <v>0</v>
+      </c>
+      <c r="EJ47">
+        <v>-17.36231960163366</v>
+      </c>
+      <c r="EK47">
+        <v>0</v>
+      </c>
+      <c r="EL47">
+        <v>2.559549231195433</v>
+      </c>
+      <c r="EM47">
+        <v>6.736624703175551</v>
+      </c>
+      <c r="EN47">
+        <v>0</v>
+      </c>
+      <c r="EO47">
+        <v>0</v>
+      </c>
+      <c r="EP47">
+        <v>0</v>
+      </c>
+      <c r="EQ47">
+        <v>0</v>
+      </c>
+      <c r="ER47">
+        <v>0</v>
+      </c>
+      <c r="ES47">
+        <v>-2.610058757624586</v>
+      </c>
+      <c r="ET47">
+        <v>22.23540089072844</v>
+      </c>
+      <c r="EU47">
+        <v>0</v>
+      </c>
+      <c r="EV47">
+        <v>0</v>
+      </c>
+      <c r="EW47">
+        <v>-0.320013916568314</v>
+      </c>
+      <c r="EX47">
+        <v>0</v>
+      </c>
+      <c r="EY47">
+        <v>0</v>
+      </c>
+      <c r="EZ47">
+        <v>0.05135207115939711</v>
+      </c>
+      <c r="FA47">
+        <v>4.679817816659863</v>
+      </c>
+      <c r="FB47">
+        <v>0</v>
+      </c>
+      <c r="FC47">
+        <v>0</v>
+      </c>
+      <c r="FD47">
+        <v>1.106913875240934</v>
+      </c>
+      <c r="FE47">
+        <v>0.01032414515469871</v>
+      </c>
+      <c r="FF47">
+        <v>0</v>
+      </c>
+      <c r="FG47">
+        <v>46.16880139988689</v>
+      </c>
+      <c r="FH47">
+        <v>0</v>
+      </c>
+      <c r="FI47">
+        <v>0</v>
+      </c>
+      <c r="FJ47">
+        <v>12.51138141524359</v>
+      </c>
+      <c r="FK47">
+        <v>0</v>
+      </c>
+      <c r="FL47">
+        <v>1.779056133720587</v>
+      </c>
+      <c r="FM47">
+        <v>0</v>
+      </c>
+      <c r="FN47">
+        <v>0</v>
+      </c>
+      <c r="FO47">
+        <v>8.014525246314463</v>
+      </c>
+      <c r="FP47">
+        <v>10.59612953715202</v>
+      </c>
+      <c r="FQ47">
+        <v>3.59570388584865</v>
+      </c>
+      <c r="FR47">
+        <v>0</v>
+      </c>
+      <c r="FS47">
+        <v>2.304506186047945</v>
+      </c>
+      <c r="FT47">
+        <v>-0.3059452754749401</v>
+      </c>
+      <c r="FU47">
+        <v>0</v>
+      </c>
+      <c r="FV47">
+        <v>0.04517168281969219</v>
+      </c>
+      <c r="FW47">
+        <v>0</v>
+      </c>
+      <c r="FX47">
+        <v>-4.032532155926219</v>
+      </c>
+      <c r="FY47">
+        <v>2.499588163234762</v>
+      </c>
+      <c r="FZ47">
+        <v>2.437686733436465</v>
+      </c>
+      <c r="GA47">
+        <v>10.60691622907962</v>
+      </c>
+      <c r="GB47">
+        <v>10.38445306631064</v>
+      </c>
+      <c r="GC47">
+        <v>0</v>
+      </c>
+      <c r="GD47">
+        <v>0</v>
+      </c>
+      <c r="GE47">
+        <v>0</v>
+      </c>
+      <c r="GF47">
+        <v>0</v>
+      </c>
+      <c r="GG47">
+        <v>0</v>
+      </c>
+      <c r="GH47">
+        <v>12.35320994870676</v>
+      </c>
+      <c r="GI47">
+        <v>1.330779943590386</v>
+      </c>
+      <c r="GJ47">
+        <v>0</v>
+      </c>
+      <c r="GK47">
+        <v>3.868687787732938</v>
+      </c>
+      <c r="GL47">
+        <v>18.92079399096087</v>
+      </c>
+      <c r="GM47">
+        <v>4.745196288303987</v>
+      </c>
+      <c r="GN47">
+        <v>0</v>
+      </c>
+      <c r="GO47">
+        <v>5.121498852822072</v>
+      </c>
+      <c r="GP47">
+        <v>2.337966704698957</v>
+      </c>
+      <c r="GQ47">
+        <v>0.1124789352095243</v>
+      </c>
+      <c r="GR47">
+        <v>0</v>
+      </c>
+      <c r="GS47">
+        <v>0</v>
+      </c>
+      <c r="GT47">
+        <v>0</v>
+      </c>
+      <c r="GU47">
+        <v>12.80132163098972</v>
+      </c>
+      <c r="GV47">
+        <v>0</v>
+      </c>
+      <c r="GW47">
+        <v>21.14173552325769</v>
+      </c>
+      <c r="GX47">
+        <v>0</v>
+      </c>
+      <c r="GY47">
+        <v>0</v>
+      </c>
+      <c r="GZ47">
+        <v>13.53522038860433</v>
+      </c>
+      <c r="HA47">
+        <v>0</v>
+      </c>
+      <c r="HB47">
+        <v>0</v>
+      </c>
+      <c r="HC47">
+        <v>0</v>
+      </c>
+      <c r="HD47">
+        <v>0.02447228491890208</v>
+      </c>
+      <c r="HE47">
+        <v>2.748281111006264</v>
+      </c>
+      <c r="HF47">
+        <v>8.225881438869692</v>
+      </c>
+      <c r="HG47">
+        <v>0</v>
+      </c>
+      <c r="HH47">
+        <v>0</v>
+      </c>
+      <c r="HI47">
+        <v>0</v>
+      </c>
+      <c r="HJ47">
+        <v>-9.562638085978961</v>
+      </c>
+      <c r="HK47">
+        <v>4.955718679490701</v>
+      </c>
+      <c r="HL47">
+        <v>2.667945642440429</v>
+      </c>
+      <c r="HM47">
+        <v>0</v>
+      </c>
+      <c r="HN47">
+        <v>0</v>
+      </c>
+      <c r="HO47">
+        <v>1.238194394947314</v>
+      </c>
+      <c r="HP47">
+        <v>0</v>
+      </c>
+      <c r="HQ47">
+        <v>60.42452968250382</v>
+      </c>
+      <c r="HR47">
+        <v>13.72900862817323</v>
+      </c>
+      <c r="HS47">
+        <v>0</v>
+      </c>
+      <c r="HT47">
+        <v>2.687140375700949</v>
+      </c>
+      <c r="HU47">
+        <v>0</v>
+      </c>
+      <c r="HV47">
+        <v>2.115556159813877</v>
+      </c>
+      <c r="HW47">
+        <v>0</v>
+      </c>
+      <c r="HX47">
+        <v>4.1450853793433</v>
+      </c>
+      <c r="HY47">
+        <v>2.168724104753551</v>
+      </c>
+      <c r="HZ47">
+        <v>0</v>
+      </c>
+      <c r="IA47">
+        <v>64.51524708733905</v>
+      </c>
+      <c r="IB47">
+        <v>17.24777301880943</v>
+      </c>
+      <c r="IC47">
+        <v>0</v>
+      </c>
+      <c r="ID47">
+        <v>0</v>
+      </c>
+      <c r="IE47">
+        <v>0.6061316550684808</v>
+      </c>
+      <c r="IF47">
+        <v>0</v>
+      </c>
+      <c r="IG47">
+        <v>0.07951605170156029</v>
+      </c>
+      <c r="IH47">
+        <v>0</v>
+      </c>
+      <c r="II47">
+        <v>28.91381123878296</v>
+      </c>
+      <c r="IJ47">
+        <v>0</v>
+      </c>
+      <c r="IK47">
+        <v>0</v>
+      </c>
+      <c r="IL47">
+        <v>0</v>
+      </c>
+      <c r="IM47">
+        <v>0</v>
+      </c>
+      <c r="IN47">
+        <v>0.3653443083019106</v>
+      </c>
+      <c r="IO47">
+        <v>2.786555496449182</v>
+      </c>
+      <c r="IP47">
+        <v>3.283650231119935</v>
+      </c>
+      <c r="IQ47">
+        <v>0</v>
+      </c>
+      <c r="IR47">
+        <v>0</v>
+      </c>
+      <c r="IS47">
+        <v>32.08437532294272</v>
+      </c>
+      <c r="IT47">
+        <v>-2.443409136816172</v>
+      </c>
+      <c r="IU47">
+        <v>3.182789288040681</v>
+      </c>
+      <c r="IV47">
+        <v>0</v>
+      </c>
+      <c r="IW47">
+        <v>16.87311744421061</v>
+      </c>
+      <c r="IX47">
+        <v>0</v>
+      </c>
+      <c r="IY47">
+        <v>4.806228152620179</v>
+      </c>
+      <c r="IZ47">
+        <v>1.241850367911979</v>
+      </c>
+      <c r="JA47">
+        <v>3.638988104308069</v>
+      </c>
+      <c r="JB47">
+        <v>48.11003940757541</v>
+      </c>
+      <c r="JC47">
+        <v>28.06494571558505</v>
+      </c>
+      <c r="JD47">
+        <v>0.04000452812339095</v>
+      </c>
+      <c r="JE47">
+        <v>-4.557673389249885</v>
+      </c>
+      <c r="JF47">
+        <v>4.281414533268844</v>
+      </c>
+      <c r="JG47">
+        <v>8.420200852132496</v>
+      </c>
+      <c r="JH47">
+        <v>0.341467418137583</v>
+      </c>
+      <c r="JI47">
+        <v>0.4134063288629477</v>
+      </c>
+      <c r="JJ47">
+        <v>0</v>
+      </c>
+      <c r="JK47">
+        <v>36.26321131768464</v>
+      </c>
+      <c r="JL47">
+        <v>0</v>
+      </c>
+      <c r="JM47">
+        <v>0</v>
+      </c>
+      <c r="JN47">
+        <v>2.228084350133997</v>
+      </c>
+      <c r="JO47">
+        <v>0</v>
+      </c>
+      <c r="JP47">
+        <v>69.6092845210419</v>
+      </c>
+      <c r="JQ47">
+        <v>0</v>
+      </c>
+      <c r="JR47">
+        <v>-0.07317037373683277</v>
+      </c>
+      <c r="JS47">
+        <v>3.99224225405419</v>
+      </c>
+      <c r="JT47">
+        <v>26.33325583540818</v>
+      </c>
+      <c r="JU47">
+        <v>16.65941073292936</v>
+      </c>
+      <c r="JV47">
+        <v>3.16277070465938</v>
+      </c>
+      <c r="JW47">
+        <v>0</v>
+      </c>
+      <c r="JX47">
+        <v>-1.84243651009848</v>
+      </c>
+      <c r="JY47">
+        <v>35.52772997703073</v>
+      </c>
+      <c r="JZ47">
+        <v>0.4463474930100233</v>
+      </c>
+      <c r="KA47">
+        <v>-0.243388704379953</v>
+      </c>
+      <c r="KB47">
+        <v>7.698266383481382</v>
+      </c>
+      <c r="KC47">
+        <v>0</v>
+      </c>
+      <c r="KD47">
+        <v>0</v>
+      </c>
+      <c r="KE47">
+        <v>8.656140379831413</v>
+      </c>
+      <c r="KF47">
+        <v>0</v>
+      </c>
+      <c r="KG47">
+        <v>-8.126878119515482</v>
+      </c>
+      <c r="KH47">
+        <v>0.4839390822741052</v>
+      </c>
+      <c r="KI47">
+        <v>0</v>
+      </c>
+      <c r="KJ47">
+        <v>0</v>
+      </c>
+      <c r="KK47">
+        <v>0</v>
+      </c>
+      <c r="KL47">
+        <v>2.085156638345111</v>
+      </c>
+      <c r="KM47">
+        <v>0.01326316314913356</v>
+      </c>
+      <c r="KN47">
+        <v>0</v>
+      </c>
+      <c r="KO47">
+        <v>1.874128976166162</v>
+      </c>
+      <c r="KP47">
+        <v>0</v>
+      </c>
+      <c r="KQ47">
+        <v>5.679945798114034</v>
+      </c>
+      <c r="KR47">
+        <v>20.96033614063731</v>
+      </c>
+      <c r="KS47">
+        <v>0</v>
+      </c>
+      <c r="KT47">
+        <v>0</v>
+      </c>
+      <c r="KU47">
+        <v>0</v>
+      </c>
+      <c r="KV47">
+        <v>4.182197204893356</v>
+      </c>
+      <c r="KW47">
+        <v>0.7346426906021009</v>
+      </c>
+      <c r="KX47">
+        <v>0.004962519801303023</v>
+      </c>
+      <c r="KY47">
+        <v>7.579631998538161</v>
+      </c>
+      <c r="KZ47">
+        <v>4.030721054415721</v>
+      </c>
+      <c r="LA47">
+        <v>-0.06632527732671178</v>
+      </c>
+      <c r="LB47">
+        <v>33.0115843254581</v>
+      </c>
+      <c r="LC47">
+        <v>2.082527446535693</v>
+      </c>
+      <c r="LD47">
+        <v>0</v>
+      </c>
+      <c r="LE47">
+        <v>0.07480146224122564</v>
+      </c>
+      <c r="LF47">
+        <v>0</v>
+      </c>
+      <c r="LG47">
+        <v>2.03623736702832</v>
+      </c>
+      <c r="LH47">
+        <v>0</v>
+      </c>
+      <c r="LI47">
+        <v>0</v>
+      </c>
+      <c r="LJ47">
+        <v>18.20167371440328</v>
+      </c>
+      <c r="LK47">
+        <v>35.78497493219777</v>
+      </c>
+      <c r="LL47">
+        <v>0.2493163912023242</v>
+      </c>
+      <c r="LM47">
+        <v>0.329735507030108</v>
+      </c>
+      <c r="LN47">
+        <v>4.055732498288705</v>
+      </c>
+      <c r="LO47">
+        <v>2.272273380858223</v>
+      </c>
+      <c r="LP47">
+        <v>0</v>
+      </c>
+      <c r="LQ47">
+        <v>6.196571735125872</v>
+      </c>
+      <c r="LR47">
+        <v>0.1878670710616888</v>
+      </c>
+      <c r="LS47">
+        <v>0</v>
+      </c>
+      <c r="LT47">
+        <v>0</v>
+      </c>
+      <c r="LU47">
+        <v>0.03934841065151673</v>
+      </c>
+      <c r="LV47">
+        <v>1.151492524779343</v>
+      </c>
+      <c r="LW47">
+        <v>81.01749659023199</v>
+      </c>
+      <c r="LX47">
+        <v>1.11823753611867</v>
+      </c>
+      <c r="LY47">
+        <v>0</v>
+      </c>
+      <c r="LZ47">
+        <v>0.225221430241926</v>
+      </c>
+      <c r="MA47">
+        <v>1.159043403789205</v>
+      </c>
+      <c r="MB47">
+        <v>41.81912345837327</v>
+      </c>
+      <c r="MC47">
+        <v>0</v>
+      </c>
+      <c r="MD47">
+        <v>0</v>
+      </c>
+      <c r="ME47">
+        <v>0</v>
+      </c>
+      <c r="MF47">
+        <v>-1.959306097516048</v>
+      </c>
+      <c r="MG47">
+        <v>50.43125979874253</v>
+      </c>
+      <c r="MH47">
+        <v>0</v>
+      </c>
+      <c r="MI47">
+        <v>-0</v>
+      </c>
+      <c r="MJ47">
+        <v>0</v>
+      </c>
+      <c r="MK47">
+        <v>0</v>
+      </c>
+      <c r="ML47">
+        <v>3.535739695869722</v>
+      </c>
+      <c r="MM47">
+        <v>0</v>
+      </c>
+      <c r="MN47">
+        <v>0.3035007166577799</v>
+      </c>
+      <c r="MO47">
+        <v>47.76981646536183</v>
+      </c>
+      <c r="MP47">
+        <v>6.686123320477719</v>
+      </c>
+      <c r="MQ47">
+        <v>46.87450368390637</v>
+      </c>
+      <c r="MR47">
+        <v>0</v>
+      </c>
+      <c r="MS47">
+        <v>9.777562093076767</v>
+      </c>
+      <c r="MT47">
+        <v>0.1238730175267051</v>
+      </c>
+      <c r="MU47">
+        <v>0</v>
+      </c>
+      <c r="MV47">
+        <v>0</v>
+      </c>
+      <c r="MW47">
+        <v>0</v>
+      </c>
+      <c r="MX47">
+        <v>0</v>
+      </c>
+      <c r="MY47">
+        <v>2.641189323312148</v>
+      </c>
+      <c r="MZ47">
+        <v>0</v>
+      </c>
+      <c r="NA47">
+        <v>0.109246662570623</v>
+      </c>
+      <c r="NB47">
+        <v>7.621615506374667</v>
+      </c>
+      <c r="NC47">
+        <v>0</v>
+      </c>
+      <c r="ND47">
+        <v>6.980425572958097</v>
+      </c>
+      <c r="NE47">
+        <v>3.68577200146342</v>
+      </c>
+      <c r="NF47">
+        <v>1.140846576378586</v>
+      </c>
+      <c r="NG47">
+        <v>24.29338005741101</v>
+      </c>
+      <c r="NH47">
+        <v>1.902729005427659</v>
+      </c>
+      <c r="NI47">
+        <v>0</v>
+      </c>
+      <c r="NJ47">
+        <v>0</v>
+      </c>
+      <c r="NK47">
+        <v>-5.852162141685881</v>
+      </c>
+      <c r="NL47">
+        <v>0</v>
+      </c>
+      <c r="NM47">
+        <v>0</v>
+      </c>
+      <c r="NN47">
+        <v>-2.808898812117377</v>
+      </c>
+      <c r="NO47">
+        <v>0</v>
+      </c>
+      <c r="NP47">
+        <v>4.735716730866955</v>
+      </c>
+      <c r="NQ47">
+        <v>9.916010074399821</v>
+      </c>
+      <c r="NR47">
+        <v>13.28426046306231</v>
+      </c>
+      <c r="NS47">
+        <v>0</v>
+      </c>
+      <c r="NT47">
+        <v>0</v>
+      </c>
+      <c r="NU47">
+        <v>0</v>
+      </c>
+      <c r="NV47">
+        <v>0.03213895108101061</v>
+      </c>
+      <c r="NW47">
+        <v>0.1331444284576846</v>
+      </c>
+      <c r="NX47">
+        <v>18.56109705514234</v>
+      </c>
+      <c r="NY47">
+        <v>0.01373058642904645</v>
+      </c>
+      <c r="NZ47">
+        <v>-16.2973955922464</v>
+      </c>
+      <c r="OA47">
+        <v>0</v>
+      </c>
+      <c r="OB47">
+        <v>15.4718271500322</v>
+      </c>
+      <c r="OC47">
+        <v>0</v>
+      </c>
+      <c r="OD47">
+        <v>0</v>
+      </c>
+      <c r="OE47">
+        <v>-2.401042571934994</v>
+      </c>
+      <c r="OF47">
+        <v>0</v>
+      </c>
+      <c r="OG47">
+        <v>0</v>
+      </c>
+      <c r="OH47">
+        <v>2.929996818911064</v>
+      </c>
+      <c r="OI47">
+        <v>0</v>
+      </c>
+      <c r="OJ47">
+        <v>1.57070369563877</v>
+      </c>
+      <c r="OK47">
+        <v>0</v>
+      </c>
+      <c r="OL47">
+        <v>0</v>
+      </c>
+      <c r="OM47">
+        <v>0</v>
+      </c>
+      <c r="ON47">
+        <v>0</v>
+      </c>
+      <c r="OO47">
+        <v>0</v>
+      </c>
+      <c r="OP47">
+        <v>0.2306361317415169</v>
+      </c>
+      <c r="OQ47">
+        <v>14.95476814511221</v>
+      </c>
+      <c r="OR47">
+        <v>0.007333998321566781</v>
+      </c>
+      <c r="OS47">
+        <v>1.0355074853139</v>
+      </c>
+      <c r="OT47">
+        <v>0</v>
+      </c>
+      <c r="OU47">
+        <v>0.6607557905098105</v>
+      </c>
+      <c r="OV47">
+        <v>0</v>
+      </c>
+      <c r="OW47">
+        <v>0.01907174127433109</v>
+      </c>
+      <c r="OX47">
+        <v>0</v>
+      </c>
+      <c r="OY47">
+        <v>32.15519289984081</v>
+      </c>
+      <c r="OZ47">
+        <v>0</v>
+      </c>
+      <c r="PA47">
+        <v>1.687445795827358</v>
+      </c>
+      <c r="PB47">
+        <v>0</v>
+      </c>
+      <c r="PC47">
+        <v>1.265070704930949</v>
+      </c>
+      <c r="PD47">
+        <v>0</v>
+      </c>
+      <c r="PE47">
+        <v>20.2065282182129</v>
+      </c>
+      <c r="PF47">
+        <v>4.210174945785525</v>
+      </c>
+      <c r="PG47">
+        <v>0</v>
+      </c>
+      <c r="PH47">
+        <v>-3.218573468129193</v>
+      </c>
+      <c r="PI47">
+        <v>3.943715871801714</v>
+      </c>
+      <c r="PJ47">
+        <v>0</v>
+      </c>
+      <c r="PK47">
+        <v>17.46141349550214</v>
+      </c>
+      <c r="PL47">
+        <v>0</v>
+      </c>
+      <c r="PM47">
+        <v>0</v>
+      </c>
+      <c r="PN47">
+        <v>-0.1895550809639275</v>
+      </c>
+      <c r="PO47">
+        <v>8.638311860984345</v>
+      </c>
+      <c r="PP47">
+        <v>10.59887978475626</v>
+      </c>
+      <c r="PQ47">
+        <v>6.013101974591819</v>
+      </c>
+      <c r="PR47">
+        <v>1.403186607079306</v>
+      </c>
+      <c r="PS47">
+        <v>0.8061222668388552</v>
+      </c>
+      <c r="PT47">
+        <v>8.54881624014439</v>
+      </c>
+      <c r="PU47">
+        <v>0</v>
+      </c>
+      <c r="PV47">
+        <v>0</v>
+      </c>
+      <c r="PW47">
+        <v>-4.321856666234282</v>
+      </c>
+      <c r="PX47">
+        <v>3.481372447755007</v>
+      </c>
+      <c r="PY47">
+        <v>0</v>
+      </c>
+      <c r="PZ47">
+        <v>0.07820352214579529</v>
+      </c>
+      <c r="QA47">
+        <v>13.7303321948902</v>
+      </c>
+      <c r="QB47">
+        <v>0</v>
+      </c>
+      <c r="QC47">
+        <v>0</v>
+      </c>
+      <c r="QD47">
+        <v>0</v>
+      </c>
+      <c r="QE47">
+        <v>3.406877505814236</v>
+      </c>
+      <c r="QF47">
+        <v>-0.001355979304939636</v>
+      </c>
+      <c r="QG47">
+        <v>0.6388854716640679</v>
+      </c>
+      <c r="QH47">
+        <v>0</v>
+      </c>
+      <c r="QI47">
+        <v>14.02384230265102</v>
+      </c>
+      <c r="QJ47">
+        <v>0</v>
+      </c>
+      <c r="QK47">
+        <v>13.36342878677908</v>
+      </c>
+      <c r="QL47">
+        <v>0.6877764559268087</v>
+      </c>
+      <c r="QM47">
+        <v>-0.004525757986332923</v>
+      </c>
+      <c r="QN47">
+        <v>3.918954110351478</v>
+      </c>
+      <c r="QO47">
+        <v>43.12969935699857</v>
+      </c>
+      <c r="QP47">
+        <v>25.72061733965666</v>
+      </c>
+      <c r="QQ47">
+        <v>6.58282300356376</v>
+      </c>
+      <c r="QR47">
+        <v>0</v>
+      </c>
+      <c r="QS47">
+        <v>0</v>
+      </c>
+      <c r="QT47">
+        <v>0</v>
+      </c>
+      <c r="QU47">
+        <v>4.53177374167079</v>
+      </c>
+      <c r="QV47">
+        <v>0</v>
+      </c>
+      <c r="QW47">
+        <v>5.537733889190633</v>
+      </c>
+      <c r="QX47">
+        <v>0</v>
+      </c>
+      <c r="QY47">
+        <v>0</v>
+      </c>
+      <c r="QZ47">
+        <v>0</v>
+      </c>
+      <c r="RA47">
+        <v>4.838480586284447</v>
+      </c>
+      <c r="RB47">
+        <v>0</v>
+      </c>
+      <c r="RC47">
+        <v>1.466331902930548</v>
+      </c>
+      <c r="RD47">
+        <v>2.830066585283987</v>
+      </c>
+      <c r="RE47">
+        <v>5.105724601786505</v>
+      </c>
+      <c r="RF47">
+        <v>0</v>
+      </c>
+      <c r="RG47">
+        <v>0</v>
+      </c>
+      <c r="RH47">
+        <v>0</v>
+      </c>
+      <c r="RI47">
+        <v>8.991837814357496</v>
+      </c>
+      <c r="RJ47">
+        <v>3.262147661126562</v>
+      </c>
+      <c r="RK47">
+        <v>4.384218087098361</v>
+      </c>
+      <c r="RL47">
+        <v>20.80010295201873</v>
+      </c>
+      <c r="RM47">
+        <v>-1.197928908976706</v>
+      </c>
+      <c r="RN47">
+        <v>0</v>
+      </c>
+      <c r="RO47">
+        <v>0</v>
+      </c>
+      <c r="RP47">
+        <v>-0.4917433900604919</v>
+      </c>
+      <c r="RQ47">
+        <v>0</v>
+      </c>
+      <c r="RR47">
+        <v>2.711827948810082</v>
       </c>
     </row>
   </sheetData>

</xml_diff>